<commit_message>
Mise à jour Projet_Learn_v1.docx et synchro dossiers
</commit_message>
<xml_diff>
--- a/ressources-externes/Local/User_Stories_et_tâches.xlsx
+++ b/ressources-externes/Local/User_Stories_et_tâches.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,10 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bernard\Documents\_OpenClassrooms\Git\Projet3-Dev4U\ressources-externes\Local\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40001_{747CFC17-CC72-4395-93AF-2AB466C311D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23BFC217-D6BC-4535-9D53-C47194AF329A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-180" yWindow="-16320" windowWidth="29040" windowHeight="16440" activeTab="1"/>
-    <workbookView xWindow="2130" yWindow="-14085" windowWidth="21600" windowHeight="11505"/>
+    <workbookView xWindow="-40" yWindow="-10780" windowWidth="10800" windowHeight="10780" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="User stories" sheetId="1" r:id="rId1"/>
@@ -27,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="94">
   <si>
     <t>Afficher les tâches</t>
   </si>
@@ -65,9 +64,6 @@
     <t>Page de tableau de bord</t>
   </si>
   <si>
-    <t>en tant qu'acteur, je veux renouveler mon mot de passe afin de pouvoir me connecter à mon esspace de travail sur le site Lear@Home</t>
-  </si>
-  <si>
     <t>En tant qu'acteur, je souhaite me connecter afin d'accéder à mon espace de travail sur le site Learn@Home</t>
   </si>
   <si>
@@ -83,15 +79,6 @@
     <t>Visualiser Tableau de bord</t>
   </si>
   <si>
-    <t>En tant que tuteur, je souhaite pouvoir créer un compte afin de pouvoir accéder à mon espace de travail sur Learn@Home</t>
-  </si>
-  <si>
-    <t>En tant qu'élève, je souhaite créer un copte afin de pouvoir accéder à mon espace de travail sur le site Learn@Home</t>
-  </si>
-  <si>
-    <t>Etant donné que je suis sur la page de login du site Lear@Home, alors je saisis mon adresse de messagerie choisie pour m'identifier alors je saisis mon mot le mot de passe associé à monidentifiant, alors je clique sur la touche entrée</t>
-  </si>
-  <si>
     <t>En tant qu'acteur, je peux sélectionner la rubrique des tâches qui me sont affectées afin d'en afficher la liste</t>
   </si>
   <si>
@@ -320,13 +307,25 @@
     <t>sdf</t>
   </si>
   <si>
-    <t>Etant donné mon emplacement sur la page de connexion du site Learn@Home,</t>
+    <t xml:space="preserve">Alors que je suis sur la page de connexion du site Learn@Home,
+1) Lorsque je clique sur le lien « Je veux m’inscrire »
+- Alors je suis redirigé vers la page de création d’un compte
+2) Lorsque je saisis mon adresse de messagerie en tant qu’identifiant
+- Alors le système vérifie le format « email » de ma saisie et m’informe avec un message d’accompagnement
+3) Lorsque je saisis un mot de passe, 
+- Alors le système m’indique la qualité de ce Mot de passe.
+4) Lorsque je saisis le mot de passe de confirmation,
+- Alors le système m’indique si les 2 Mot de passe correspondent ou non
+5) Lorsque je clique sur le bouton Valider
+- Alors le système me confirme la création de mon compte
+- Alors le système envoie un message de confirmation sur l’adresse de messagerie indiquée comme identifiant de connexion
+- Alors le système me ramène à la page de connexion. </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -424,7 +423,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
@@ -455,6 +454,612 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1362075</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="3067050" cy="1943100"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="ZoneTexte 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3DF1DD8F-E703-6929-2450-83021CB83862}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1362075" y="523875"/>
+          <a:ext cx="3067050" cy="1943100"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="fr-FR" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>714375</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1237615</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>53340</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="Zone de texte 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4F79CD63-3587-9E2F-9611-94EA2F441E3D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1">
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="714375" y="485775"/>
+          <a:ext cx="4466590" cy="3206115"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr rot="0" vert="horz" wrap="square" lIns="91440" tIns="45720" rIns="91440" bIns="45720" anchor="t" anchorCtr="0">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:lnSpc>
+              <a:spcPct val="107000"/>
+            </a:lnSpc>
+            <a:spcAft>
+              <a:spcPts val="800"/>
+            </a:spcAft>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1100" b="1" kern="100">
+              <a:effectLst/>
+              <a:latin typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+              <a:ea typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:rPr>
+            <a:t>Alors que je</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1100" kern="100">
+              <a:effectLst/>
+              <a:latin typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+              <a:ea typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:rPr>
+            <a:t> suis sur la page de connexion du site Learn@Home,</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="342900" lvl="0" indent="-342900">
+            <a:lnSpc>
+              <a:spcPct val="107000"/>
+            </a:lnSpc>
+            <a:buFont typeface="+mj-lt"/>
+            <a:buAutoNum type="arabicParenR"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1100" b="1" kern="100">
+              <a:effectLst/>
+              <a:latin typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+              <a:ea typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:rPr>
+            <a:t>Lorsque </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1100" kern="100">
+              <a:effectLst/>
+              <a:latin typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+              <a:ea typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:rPr>
+            <a:t>je</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1100" b="1" kern="100">
+              <a:effectLst/>
+              <a:latin typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+              <a:ea typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:rPr>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1100" kern="100">
+              <a:effectLst/>
+              <a:latin typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+              <a:ea typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:rPr>
+            <a:t>clique sur le lien « Je veux m’inscrire »</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="342900" lvl="0" indent="-342900">
+            <a:lnSpc>
+              <a:spcPct val="107000"/>
+            </a:lnSpc>
+            <a:buFont typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+            <a:buChar char="-"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1100" b="1" kern="100">
+              <a:effectLst/>
+              <a:latin typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+              <a:ea typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:rPr>
+            <a:t>Alors </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1100" kern="100">
+              <a:effectLst/>
+              <a:latin typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+              <a:ea typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:rPr>
+            <a:t>je suis redirigé vers la page de création d’un compte</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="342900" lvl="0" indent="-342900">
+            <a:lnSpc>
+              <a:spcPct val="107000"/>
+            </a:lnSpc>
+            <a:buFont typeface="+mj-lt"/>
+            <a:buAutoNum type="arabicParenR"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1100" b="1" kern="100">
+              <a:effectLst/>
+              <a:latin typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+              <a:ea typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:rPr>
+            <a:t>Lorsque </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1100" kern="100">
+              <a:effectLst/>
+              <a:latin typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+              <a:ea typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:rPr>
+            <a:t>je</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1100" b="1" kern="100">
+              <a:effectLst/>
+              <a:latin typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+              <a:ea typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:rPr>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1100" kern="100">
+              <a:effectLst/>
+              <a:latin typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+              <a:ea typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:rPr>
+            <a:t>saisis mon adresse de messagerie en tant qu’identifiant</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="342900" lvl="0" indent="-342900">
+            <a:lnSpc>
+              <a:spcPct val="107000"/>
+            </a:lnSpc>
+            <a:buFont typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+            <a:buChar char="-"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1100" b="1" kern="100">
+              <a:effectLst/>
+              <a:latin typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+              <a:ea typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:rPr>
+            <a:t>Alors le système </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1100" kern="100">
+              <a:effectLst/>
+              <a:latin typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+              <a:ea typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:rPr>
+            <a:t>vérifie le format « email » de</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1100" b="1" kern="100">
+              <a:effectLst/>
+              <a:latin typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+              <a:ea typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:rPr>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1100" kern="100">
+              <a:effectLst/>
+              <a:latin typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+              <a:ea typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:rPr>
+            <a:t>ma saisie et m’informe avec un message d’accompagnement</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="342900" lvl="0" indent="-342900">
+            <a:lnSpc>
+              <a:spcPct val="107000"/>
+            </a:lnSpc>
+            <a:buFont typeface="+mj-lt"/>
+            <a:buAutoNum type="arabicParenR"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1100" b="1" kern="100">
+              <a:effectLst/>
+              <a:latin typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+              <a:ea typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:rPr>
+            <a:t>Lorsque </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1100" kern="100">
+              <a:effectLst/>
+              <a:latin typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+              <a:ea typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:rPr>
+            <a:t>je saisis un mot de passe,</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1100" b="1" kern="100">
+              <a:effectLst/>
+              <a:latin typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+              <a:ea typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:rPr>
+            <a:t> </a:t>
+          </a:r>
+          <a:endParaRPr lang="fr-FR" sz="1100" kern="100">
+            <a:effectLst/>
+            <a:latin typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+            <a:ea typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+            <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr marL="342900" lvl="0" indent="-342900">
+            <a:lnSpc>
+              <a:spcPct val="107000"/>
+            </a:lnSpc>
+            <a:buFont typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+            <a:buChar char="-"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1100" b="1" kern="100">
+              <a:effectLst/>
+              <a:latin typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+              <a:ea typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:rPr>
+            <a:t>Alors le système </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1100" kern="100">
+              <a:effectLst/>
+              <a:latin typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+              <a:ea typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:rPr>
+            <a:t>m’indique la qualité de ce Mot de passe</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1100" b="1" kern="100">
+              <a:effectLst/>
+              <a:latin typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+              <a:ea typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:rPr>
+            <a:t>.</a:t>
+          </a:r>
+          <a:endParaRPr lang="fr-FR" sz="1100" kern="100">
+            <a:effectLst/>
+            <a:latin typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+            <a:ea typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+            <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr marL="342900" lvl="0" indent="-342900">
+            <a:lnSpc>
+              <a:spcPct val="107000"/>
+            </a:lnSpc>
+            <a:buFont typeface="+mj-lt"/>
+            <a:buAutoNum type="arabicParenR"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1100" b="1" kern="100">
+              <a:effectLst/>
+              <a:latin typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+              <a:ea typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:rPr>
+            <a:t>Lorsque </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1100" kern="100">
+              <a:effectLst/>
+              <a:latin typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+              <a:ea typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:rPr>
+            <a:t>je saisis le mot de passe de confirmation,</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="342900" lvl="0" indent="-342900">
+            <a:lnSpc>
+              <a:spcPct val="107000"/>
+            </a:lnSpc>
+            <a:buFont typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+            <a:buChar char="-"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1100" b="1" kern="100">
+              <a:effectLst/>
+              <a:latin typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+              <a:ea typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:rPr>
+            <a:t>Alors le système</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1100" kern="100">
+              <a:effectLst/>
+              <a:latin typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+              <a:ea typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:rPr>
+            <a:t> m’indique si les 2 </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1100" b="1" kern="100">
+              <a:effectLst/>
+              <a:latin typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+              <a:ea typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:rPr>
+            <a:t>Mot de passe</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1100" kern="100">
+              <a:effectLst/>
+              <a:latin typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+              <a:ea typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:rPr>
+            <a:t> correspondent ou non</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="342900" lvl="0" indent="-342900">
+            <a:lnSpc>
+              <a:spcPct val="107000"/>
+            </a:lnSpc>
+            <a:buFont typeface="+mj-lt"/>
+            <a:buAutoNum type="arabicParenR"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1100" b="1" kern="100">
+              <a:effectLst/>
+              <a:latin typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+              <a:ea typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:rPr>
+            <a:t>Lorsque</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1100" kern="100">
+              <a:effectLst/>
+              <a:latin typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+              <a:ea typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:rPr>
+            <a:t> je clique sur le bouton </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1100" b="1" kern="100">
+              <a:effectLst/>
+              <a:latin typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+              <a:ea typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:rPr>
+            <a:t>Valider</a:t>
+          </a:r>
+          <a:endParaRPr lang="fr-FR" sz="1100" kern="100">
+            <a:effectLst/>
+            <a:latin typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+            <a:ea typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+            <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr marL="342900" lvl="0" indent="-342900">
+            <a:lnSpc>
+              <a:spcPct val="107000"/>
+            </a:lnSpc>
+            <a:buFont typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+            <a:buChar char="-"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1100" b="1" kern="100">
+              <a:effectLst/>
+              <a:latin typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+              <a:ea typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:rPr>
+            <a:t>Alors le système</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1100" kern="100">
+              <a:effectLst/>
+              <a:latin typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+              <a:ea typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:rPr>
+            <a:t> me confirme la création de mon compte</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="342900" lvl="0" indent="-342900">
+            <a:lnSpc>
+              <a:spcPct val="107000"/>
+            </a:lnSpc>
+            <a:buFont typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+            <a:buChar char="-"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1100" b="1" kern="100">
+              <a:effectLst/>
+              <a:latin typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+              <a:ea typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:rPr>
+            <a:t>Alors le système</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1100" kern="100">
+              <a:effectLst/>
+              <a:latin typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+              <a:ea typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:rPr>
+            <a:t> envoie un message de confirmation sur l’adresse de messagerie indiquée comme identifiant de connexion</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="342900" lvl="0" indent="-342900">
+            <a:lnSpc>
+              <a:spcPct val="107000"/>
+            </a:lnSpc>
+            <a:spcAft>
+              <a:spcPts val="800"/>
+            </a:spcAft>
+            <a:buFont typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+            <a:buChar char="-"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1100" b="1" kern="100">
+              <a:effectLst/>
+              <a:latin typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+              <a:ea typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:rPr>
+            <a:t>Alors le système</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1100" kern="100">
+              <a:effectLst/>
+              <a:latin typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+              <a:ea typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:rPr>
+            <a:t> me ramène à la page de connexion. </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr>
+            <a:lnSpc>
+              <a:spcPct val="107000"/>
+            </a:lnSpc>
+            <a:spcAft>
+              <a:spcPts val="800"/>
+            </a:spcAft>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1100" kern="100">
+              <a:effectLst/>
+              <a:latin typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+              <a:ea typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:rPr>
+            <a:t> </a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -753,14 +1358,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C4"/>
-    </sheetView>
-    <sheetView tabSelected="1" workbookViewId="1">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -773,68 +1375,65 @@
   <sheetData>
     <row r="1" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="E1" s="6" t="s">
         <v>85</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="F1" s="6" t="s">
         <v>86</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="G1" s="6" t="s">
         <v>87</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="H1" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="I1" s="6" t="s">
         <v>89</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="J1" s="6" t="s">
         <v>90</v>
-      </c>
-      <c r="G1" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="H1" s="6" t="s">
-        <v>92</v>
-      </c>
-      <c r="I1" s="6" t="s">
-        <v>93</v>
-      </c>
-      <c r="J1" s="6" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="2" spans="1:10" s="8" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
     </row>
     <row r="3" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="8" t="s">
-        <v>97</v>
-      </c>
       <c r="B3" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -842,13 +1441,13 @@
         <v>7</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
     <row r="5" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -859,10 +1458,10 @@
         <v>0</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
     </row>
     <row r="6" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -870,13 +1469,13 @@
         <v>8</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
     </row>
     <row r="7" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -884,13 +1483,13 @@
         <v>8</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
     </row>
     <row r="8" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -898,13 +1497,13 @@
         <v>8</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
     </row>
     <row r="9" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -912,13 +1511,13 @@
         <v>8</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
     <row r="10" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -926,13 +1525,13 @@
         <v>8</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
     </row>
     <row r="11" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -940,13 +1539,13 @@
         <v>9</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
     <row r="12" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -957,10 +1556,10 @@
         <v>1</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
     </row>
     <row r="13" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -968,13 +1567,13 @@
         <v>9</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="14" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -985,10 +1584,10 @@
         <v>2</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
     </row>
     <row r="15" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -996,18 +1595,18 @@
         <v>10</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
     </row>
     <row r="16" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="8" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="B16" s="4" t="s">
         <v>10</v>
@@ -1016,10 +1615,10 @@
         <v>3</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="17" spans="1:19" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -1030,10 +1629,10 @@
         <v>4</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
     </row>
     <row r="18" spans="1:19" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -1044,10 +1643,10 @@
         <v>5</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
     </row>
     <row r="19" spans="1:19" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -1058,10 +1657,10 @@
         <v>6</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.25">
@@ -1070,82 +1669,82 @@
         <v>11</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="F20" s="8" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
+        <v>26</v>
+      </c>
+      <c r="B22" t="s">
+        <v>27</v>
+      </c>
+      <c r="C22" t="s">
+        <v>28</v>
+      </c>
+      <c r="D22" t="s">
+        <v>29</v>
+      </c>
+      <c r="E22" t="s">
         <v>30</v>
       </c>
-      <c r="B22" t="s">
+      <c r="F22" t="s">
         <v>31</v>
       </c>
-      <c r="C22" t="s">
+      <c r="G22" t="s">
         <v>32</v>
       </c>
-      <c r="D22" t="s">
+      <c r="H22" t="s">
         <v>33</v>
       </c>
-      <c r="E22" t="s">
+      <c r="I22" t="s">
         <v>34</v>
       </c>
-      <c r="F22" t="s">
+      <c r="J22" t="s">
         <v>35</v>
       </c>
-      <c r="G22" t="s">
+      <c r="K22" t="s">
         <v>36</v>
       </c>
-      <c r="H22" t="s">
+      <c r="L22" t="s">
         <v>37</v>
       </c>
-      <c r="I22" t="s">
+      <c r="M22" t="s">
         <v>38</v>
       </c>
-      <c r="J22" t="s">
+      <c r="N22" t="s">
         <v>39</v>
       </c>
-      <c r="K22" t="s">
+      <c r="O22" t="s">
         <v>40</v>
       </c>
-      <c r="L22" t="s">
+      <c r="P22" t="s">
         <v>41</v>
       </c>
-      <c r="M22" t="s">
+      <c r="Q22" t="s">
         <v>42</v>
       </c>
-      <c r="N22" t="s">
+      <c r="R22" t="s">
         <v>43</v>
       </c>
-      <c r="O22" t="s">
+      <c r="S22" t="s">
         <v>44</v>
-      </c>
-      <c r="P22" t="s">
-        <v>45</v>
-      </c>
-      <c r="Q22" t="s">
-        <v>46</v>
-      </c>
-      <c r="R22" t="s">
-        <v>47</v>
-      </c>
-      <c r="S22" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="23" spans="1:19" ht="60" x14ac:dyDescent="0.25">
       <c r="B23" s="7"/>
       <c r="C23" s="7"/>
       <c r="D23" s="9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E23" s="7"/>
       <c r="F23" s="7"/>
@@ -1165,7 +1764,7 @@
     </row>
     <row r="24" spans="1:19" ht="90" x14ac:dyDescent="0.25">
       <c r="D24" s="10" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
     </row>
   </sheetData>
@@ -1175,18 +1774,16 @@
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
-    <sheetView workbookViewId="1">
-      <selection activeCell="B1" sqref="B1:B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1197,23 +1794,9 @@
     <col min="4" max="4" width="110.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>20</v>
+    <row r="1" spans="1:1" ht="195" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
+        <v>93</v>
       </c>
     </row>
   </sheetData>

</xml_diff>